<commit_message>
updated exporter to support level structure when sending to gamebust
</commit_message>
<xml_diff>
--- a/data/exported1.xlsx
+++ b/data/exported1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="campaigns" sheetId="1" state="visible" r:id="rId1"/>
@@ -583,10 +583,13 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
+  <cols>
+    <col width="16.296875" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -746,7 +749,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
@@ -891,7 +894,7 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:O5"/>
     </sheetView>
   </sheetViews>
@@ -940,7 +943,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1024,6 +1027,11 @@
           <t>failure_next</t>
         </is>
       </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Unnamed: 15</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1069,6 +1077,9 @@
       <c r="L2" t="n">
         <v>10</v>
       </c>
+      <c r="M2" t="n">
+        <v>2</v>
+      </c>
       <c r="N2" t="n">
         <v>10080</v>
       </c>
@@ -1117,8 +1128,14 @@
       <c r="L3" t="n">
         <v>10</v>
       </c>
+      <c r="M3" t="n">
+        <v>3</v>
+      </c>
       <c r="N3" t="n">
         <v>10080</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1126,7 +1143,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1135,7 +1152,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>G2</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1165,8 +1182,14 @@
       <c r="L4" t="n">
         <v>10</v>
       </c>
+      <c r="M4" t="n">
+        <v>4</v>
+      </c>
       <c r="N4" t="n">
         <v>10080</v>
+      </c>
+      <c r="O4" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -1174,7 +1197,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1183,7 +1206,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>G3</t>
+          <t>G4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1213,8 +1236,14 @@
       <c r="L5" t="n">
         <v>10</v>
       </c>
+      <c r="M5" t="n">
+        <v>5</v>
+      </c>
       <c r="N5" t="n">
         <v>10080</v>
+      </c>
+      <c r="O5" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -1222,7 +1251,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1231,7 +1260,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>G4</t>
+          <t>G5</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1261,8 +1290,14 @@
       <c r="L6" t="n">
         <v>10</v>
       </c>
+      <c r="M6" t="n">
+        <v>6</v>
+      </c>
       <c r="N6" t="n">
         <v>10080</v>
+      </c>
+      <c r="O6" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -1270,7 +1305,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1279,7 +1314,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>G4</t>
+          <t>G6</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1309,8 +1344,14 @@
       <c r="L7" t="n">
         <v>10</v>
       </c>
+      <c r="M7" t="n">
+        <v>7</v>
+      </c>
       <c r="N7" t="n">
         <v>10080</v>
+      </c>
+      <c r="O7" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -1318,7 +1359,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1327,7 +1368,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>G5</t>
+          <t>G7</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1357,8 +1398,14 @@
       <c r="L8" t="n">
         <v>10</v>
       </c>
+      <c r="M8" t="n">
+        <v>8</v>
+      </c>
       <c r="N8" t="n">
         <v>10080</v>
+      </c>
+      <c r="O8" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -1366,7 +1413,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1375,7 +1422,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>G6</t>
+          <t>G8</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1408,53 +1455,8 @@
       <c r="N9" t="n">
         <v>10080</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>17</v>
-      </c>
-      <c r="B10" t="n">
-        <v>6</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>G6</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G10" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H10" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I10" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>10</v>
-      </c>
-      <c r="N10" t="n">
-        <v>10080</v>
+      <c r="O9" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1468,7 +1470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1583,7 +1585,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, r0yavu9s8svq9d02jylsuewjapg729l34plgpji5311mkkv]</t>
+          <t>[SECRET, EQUAL, zwlcdg9mhu9m22271]</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -1601,7 +1603,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Take a 15-minute walk without stopping.</t>
+          <t>Run 500 km.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1630,7 +1632,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, 3w7e5j8zahfjh4t4lgnc9pdso92s]</t>
+          <t>[SECRET, EQUAL, dueo51fidkf6sphdyrsc9d9ti7ctf0iozc129ru2m9czs151l]</t>
         </is>
       </c>
       <c r="M3" t="n">
@@ -1677,7 +1679,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, e5o8go1jg759c1b47pcnkota]</t>
+          <t>[SECRET, EQUAL, hgf6r426olnjbjc6pg8u7g0o4rj2vn0h9026v2vigqfsg5plp]</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -1695,7 +1697,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Take a 15-minute walk without stopping.</t>
+          <t>Put on your walking shoes and take a picture of them.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1704,7 +1706,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
         <v>7</v>
@@ -1724,7 +1726,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, atfjqgd7wacq2b37oidbv4xgmkrcobva63raj0zmu]</t>
+          <t>[SECRET, EQUAL, pf87yebsshdegb0xxe6jw52rijnh]</t>
         </is>
       </c>
       <c r="M5" t="n">
@@ -1771,7 +1773,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, jcw87ky30j]</t>
+          <t>[SECRET, EQUAL, 7w08gj5f350tikr76jehm93q7uc4qulrea2gjml70]</t>
         </is>
       </c>
       <c r="M6" t="n">
@@ -1818,7 +1820,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, yeao98o4s44npim6ebpjwpn9pcn5owftjc]</t>
+          <t>[SECRET, EQUAL, vvzbllfdhys320pj4g8rp2wagx8pb5fjzyg5zhgxqidkba]</t>
         </is>
       </c>
       <c r="M7" t="n">
@@ -1865,7 +1867,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, 0pibs17ar8m3we4214ozrxuqont9kwck2wcn36ib2koe]</t>
+          <t>[SECRET, EQUAL, fw5efp0oo2vt1qyzbwz9bmi82wsmvdo8rogs0tf8w6ubr]</t>
         </is>
       </c>
       <c r="M8" t="n">
@@ -1883,7 +1885,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Call a friend</t>
+          <t>Go to a social event</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1892,7 +1894,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
         <v>7</v>
@@ -1912,7 +1914,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, q20hz6qakaml5rrcjpseaedx7neig91528n6bq4i]</t>
+          <t>[SECRET, EQUAL, 7o9fxz5b4sj]</t>
         </is>
       </c>
       <c r="M9" t="n">
@@ -1926,11 +1928,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Engage with others</t>
+          <t>tutorial_video(cognitive, counter)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1959,13 +1961,60 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, xot14bgk5djjwpxkskkaw1bxkgz720z0g666j]</t>
+          <t>[SECRET, EQUAL, ogv5mr71lewv8gw02oip3suu98t4p7y8byadk4z]</t>
         </is>
       </c>
       <c r="M10" t="n">
         <v>1</v>
       </c>
       <c r="N10" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Play a boardgame</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>[SECRET, EQUAL, ugph2esb05]</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="inlineStr">
         <is>
           <t>GameBus Studio</t>
         </is>
@@ -2041,7 +2090,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>

</xml_diff>

<commit_message>
added h5p links hardcoded
</commit_message>
<xml_diff>
--- a/data/exported1.xlsx
+++ b/data/exported1.xlsx
@@ -1070,7 +1070,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
         <v>2</v>
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M3" t="n">
         <v>3</v>
@@ -1175,7 +1175,7 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
         <v>4</v>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
         <v>6</v>
@@ -1337,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M7" t="n">
         <v>7</v>
@@ -1391,7 +1391,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
         <v>8</v>
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N9" t="n">
         <v>10080</v>
@@ -1465,7 +1465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1559,6 +1559,11 @@
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/a4466cf8-adb1-4a54-9e56-075eae837a53.h5p</t>
+        </is>
+      </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
@@ -1567,12 +1572,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -1580,7 +1585,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, zhrm3is3d5erba3]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 41tjqwea1ffyckchzk1nbgh70bcd5ude0mfzo044h5]</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -1627,11 +1632,11 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, n3a5q2e6w3zhtsycxg66ob4telfoj3f2ha]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, y3soyvr6b7ba257d6drh8vhao92hhss]</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -1653,6 +1658,11 @@
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/a4466cf8-adb1-4a54-9e56-075eae837a53.h5p</t>
+        </is>
+      </c>
       <c r="G4" t="n">
         <v>1</v>
       </c>
@@ -1661,12 +1671,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -1674,7 +1684,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, 2b8jocfnew1wypxd9pl686xn8gdf1yb]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 8v7zcqxdoh2y1rgv03x0mp85twljp9vv3zuq]</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -1692,7 +1702,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Take_300_steps</t>
+          <t>Complete_this_7-minute_workout_</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1708,12 +1718,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K5" t="n">
@@ -1721,11 +1731,11 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 4000]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, xnxb8ord0e0lbi1k66uj]</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -1747,6 +1757,11 @@
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/f0a366cc-c574-4807-8dab-5dd53dd47f70.h5p</t>
+        </is>
+      </c>
       <c r="G6" t="n">
         <v>1</v>
       </c>
@@ -1755,12 +1770,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="K6" t="n">
@@ -1768,7 +1783,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, yeyoh5kd5p647vmb63ech4lef3je9qc64xp9]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, vkg1bnwds948gnu1v]</t>
         </is>
       </c>
       <c r="M6" t="n">
@@ -1786,7 +1801,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Engage_with_others</t>
+          <t>Call_a_friend</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1815,7 +1830,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, g8dcx4j2tffo4mrrdiu0fs8pv8fs0dd6g1skbddolc13v5dn]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, vpukujc121qruri114neexxjca]</t>
         </is>
       </c>
       <c r="M7" t="n">
@@ -1829,11 +1844,11 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>tutorial_video(cognitive_activity)</t>
+          <t>Engage_with_others</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1862,11 +1877,11 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, zq1rro3hu94p]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 56vbpv46pi6o0kd1qswe62vz6he]</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -1876,11 +1891,11 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Do_a_5_min_yoga_session</t>
+          <t>Call_a_friend</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1909,7 +1924,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, kq3w0i7lb1jzylsf9hxgabshe5gxwbygm]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, x6at4dk676y2wn5py15f6wwrx9b78rwcvwxjf2e948fuo]</t>
         </is>
       </c>
       <c r="M9" t="n">
@@ -1923,16 +1938,21 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Do_a_5_min_yoga_session</t>
+          <t>tutorial_video(cognitive_activity)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/66972617-5cd5-40e1-8432-ecd99b7dcf10.h5p</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -1943,12 +1963,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="K10" t="n">
@@ -1956,13 +1976,60 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[SECRET, EQUAL, fj714u3fn1c3l28plk]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 211u6257haj866jm15zsuq5mnu86knjxk]</t>
         </is>
       </c>
       <c r="M10" t="n">
         <v>1</v>
       </c>
       <c r="N10" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Play_a_boardgame</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, ag59egygi2bk06ritq8bz7nbnbf276cf2ej1]</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>4</v>
+      </c>
+      <c r="N11" t="inlineStr">
         <is>
           <t>GameBus Studio</t>
         </is>

</xml_diff>

<commit_message>
cleanup + added activities
</commit_message>
<xml_diff>
--- a/data/exported1.xlsx
+++ b/data/exported1.xlsx
@@ -943,7 +943,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="M3" t="n">
         <v>3</v>
@@ -1231,119 +1231,11 @@
       <c r="L5" t="n">
         <v>4</v>
       </c>
-      <c r="M5" t="n">
-        <v>5</v>
-      </c>
       <c r="N5" t="n">
         <v>10080</v>
       </c>
       <c r="O5" t="n">
         <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>17</v>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>G5</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G6" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H6" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I6" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>6</v>
-      </c>
-      <c r="N6" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O6" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>17</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>G6</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H7" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I7" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>4</v>
-      </c>
-      <c r="N7" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O7" t="n">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1357,7 +1249,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1477,7 +1369,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, qxotnd0avuuekrmbca]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, o5bnwon9i6rv3nupuntgzsqhywfb0sk7sppsi9mazy5bwu5ph]</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -1495,7 +1387,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Do_10_push-ups</t>
+          <t>Take_a_45-minute_walk_without_stopping</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1524,7 +1416,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, re19wyg09q806txjs15lw2o00etdmych6mmjnjusfx1w]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 60szg8o5o8]</t>
         </is>
       </c>
       <c r="M3" t="n">
@@ -1542,7 +1434,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Do_10_push-ups</t>
+          <t>Take_200_steps</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1558,12 +1450,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -1571,11 +1463,11 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, t1bcmywi92srzqybmy8c648hpd44]</t>
+          <t>[STEPS, STRICTLY_GREATER, 3000], [SECRET, EQUAL, ej3dg5z2rq1m6g7v97m]</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -1585,21 +1477,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>tutorial_video(social_activity)</t>
+          <t>Include_10_minutes_of_uphill_walking_during_one_of_your_walks</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/f0a366cc-c574-4807-8dab-5dd53dd47f70.h5p</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -1610,12 +1497,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K5" t="n">
@@ -1623,11 +1510,11 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, oybwxuwyitecc27rbn2xapwa9lmiml9]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, h6xgwwhtqnc2gplsy3h1ncqvt09bssdiqxi6rk8cjk9ku8u]</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -1637,11 +1524,11 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Engage_with_others</t>
+          <t>Walk_9000_steps_in_a_day</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1657,12 +1544,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>DAY_AGGREGATE</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>DAY_AGGREGATE</t>
         </is>
       </c>
       <c r="K6" t="n">
@@ -1670,11 +1557,11 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 6u0r0owl0iehx57xczcoc6dxwc7fkaeg155]</t>
+          <t>[STEPS_SUM, STRICTLY_GREATER, 9000], [SECRET, EQUAL, 1aaukm7ml4g9m8]</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -1684,21 +1571,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>tutorial_video(cognitive_activity)</t>
+          <t>Walk_9000_steps_in_a_day</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/66972617-5cd5-40e1-8432-ecd99b7dcf10.h5p</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -1709,12 +1591,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>DAY_AGGREGATE</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>DAY_AGGREGATE</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -1722,11 +1604,11 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, f5lzxrr43rpe4vyba3xt5uusnz00vpfsyek1a1n2h]</t>
+          <t>[STEPS_SUM, STRICTLY_GREATER, 9000], [SECRET, EQUAL, qqj1vx1hq6ndxp5d6q907icqb1zeeh1t7vj81fvypxm]</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -1736,16 +1618,21 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Play_a_boardgame</t>
+          <t>tutorial_video(social_activity)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/f0a366cc-c574-4807-8dab-5dd53dd47f70.h5p</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1756,12 +1643,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="K8" t="n">
@@ -1769,13 +1656,154 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, q35dre9hwrz7w74rsv9mrhk16ec8kh48jg9mv9bh0ahocan]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, dibhlux6stuurubsixtsfnfa5nke6v5kr]</t>
         </is>
       </c>
       <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>4</v>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Call_a_friend</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>7</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, 81hceada27ud7qcheqdudbuaqkb]</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Go_to_a_social_event</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>7</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, fa5e6ynirrcd]</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>2</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Call_a_friend</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, 75lkfq7psmamjg9q65xdy]</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="inlineStr">
         <is>
           <t>GameBus Studio</t>
         </is>

</xml_diff>